<commit_message>
fix issue 38 (#40)
updated reference files
</commit_message>
<xml_diff>
--- a/src/zdemo_excel_comments.w3mi.data.xlsx
+++ b/src/zdemo_excel_comments.w3mi.data.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>ROSSIS</author>
+    <author>DEVELOPER</author>
   </authors>
   <commentList>
     <comment ref="B13" authorId="0">
@@ -49,6 +49,21 @@
         </r>
       </text>
     </comment>
+    <comment ref="F6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">A comment split
+on 2 lines?</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -56,7 +71,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>ROSSIS</author>
+    <author>DEVELOPER</author>
   </authors>
   <commentList>
     <comment ref="A8" authorId="0">

</xml_diff>